<commit_message>
Sync flatfiles from remote location
</commit_message>
<xml_diff>
--- a/scripts/flat-files/SailingPackages/SailingPackage.xlsx
+++ b/scripts/flat-files/SailingPackages/SailingPackage.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://celestyalepe.sharepoint.com/sites/CommercialExcellence-ToolingTech/Shared Documents/General/6. File_Share/Web Cache/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_BC4EB32AFE82BCE1C851F3599A4DF0B49E5EEC3C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D29A593D-4B2C-409A-90ED-983BC91F7A41}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_BC4EB32AFE82BCE1C851F3599A4DF0B49E5EEC3C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDBBEE09-35CD-497E-8318-3DF4FBBBCFC4}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$35</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="42">
   <si>
     <t>PortFrom</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Required</t>
   </si>
   <si>
-    <t>ABU</t>
-  </si>
-  <si>
     <t>ABDF125</t>
   </si>
   <si>
@@ -162,6 +159,12 @@
   </si>
   <si>
     <t>S ADRIATIC AND IDYLLIC</t>
+  </si>
+  <si>
+    <t>ABD</t>
+  </si>
+  <si>
+    <t>7NARABIANICONDXB</t>
   </si>
 </sst>
 </file>
@@ -550,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC35"/>
+  <dimension ref="A1:BC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,16 +586,16 @@
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -639,16 +642,16 @@
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -656,16 +659,16 @@
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -673,16 +676,16 @@
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -690,16 +693,16 @@
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -707,16 +710,16 @@
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -724,16 +727,16 @@
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -741,16 +744,16 @@
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C9">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -758,16 +761,16 @@
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -775,16 +778,16 @@
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -792,16 +795,16 @@
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -809,16 +812,16 @@
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -826,16 +829,16 @@
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -843,16 +846,16 @@
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -860,16 +863,16 @@
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -877,16 +880,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -894,16 +897,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -911,16 +914,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -928,16 +931,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -945,16 +948,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -962,16 +965,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22">
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -979,16 +982,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -996,16 +999,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1013,16 +1016,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1030,16 +1033,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1047,16 +1050,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1064,16 +1067,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1081,16 +1084,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1098,16 +1101,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1115,16 +1118,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1132,16 +1135,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32">
         <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1149,16 +1152,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33">
         <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1166,16 +1169,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34">
         <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1183,22 +1186,57 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35">
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
     </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E35" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1433,6 +1471,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8ccb410-e8f8-4e64-923b-36eaccbbdce1">
@@ -1441,15 +1488,6 @@
     <TaxCatchAll xmlns="1f0d39c8-c576-416d-9b8e-2dcd71db641c" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1472,6 +1510,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5461E57B-1E5F-4E65-A945-C8A202A07209}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D61AE56-39B0-4970-B18D-D4B1AB4585EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1480,12 +1526,4 @@
     <ds:schemaRef ds:uri="1f0d39c8-c576-416d-9b8e-2dcd71db641c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5461E57B-1E5F-4E65-A945-C8A202A07209}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>